<commit_message>
Costs not in M$ but in $
</commit_message>
<xml_diff>
--- a/data/desalination_costs.xlsx
+++ b/data/desalination_costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Projects/Kenya2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E25A1D-DCB8-FF4F-A415-CE136B400D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6484F246-BEEC-E447-BC47-4D52E89CF832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1573,13 +1573,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.071882007306125</c:v>
+                  <c:v>13.071882007306126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3729120029701063</c:v>
+                  <c:v>13.372912002970107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4698220159781634</c:v>
+                  <c:v>13.469822015978163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1933,13 +1933,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.3010299956639813</c:v>
+                  <c:v>14.301029995663981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6020599913279625</c:v>
+                  <c:v>14.602059991327963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6672918943003445</c:v>
+                  <c:v>14.667291894300345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4469,15 +4469,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>521608</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>603251</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>458108</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>539751</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4770,7 +4770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -5314,8 +5314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C8F88-4382-4F4A-9CA7-C097F9CC2787}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5465,12 +5465,12 @@
         <v>76.033057851239676</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G11" si="1">H3</f>
-        <v>20</v>
+        <f>H3*1000000</f>
+        <v>20000000</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H11" si="2">G9*(1-0.41)</f>
-        <v>11.8</v>
+        <f>G9*(1-0.41)</f>
+        <v>11800000.000000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5483,12 +5483,12 @@
         <v>305.78512396694219</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" ref="G10:G11" si="1">H4*1000000</f>
+        <v>40000000</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>23.6</v>
+        <f t="shared" ref="H9:H11" si="2">G10*(1-0.41)</f>
+        <v>23600000.000000004</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -5502,11 +5502,11 @@
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>50000000</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>29.500000000000004</v>
+        <v>29500000.000000004</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -5524,7 +5524,7 @@
       </c>
       <c r="F14">
         <f>LOG(H9*1000000)</f>
-        <v>7.071882007306125</v>
+        <v>13.071882007306126</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:F16" si="4">LOG(H10*1000000)</f>
-        <v>7.3729120029701063</v>
+        <v>13.372912002970107</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -5544,7 +5544,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>7.4698220159781634</v>
+        <v>13.469822015978163</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -5663,7 +5663,7 @@
         <v>26.950354609929079</v>
       </c>
       <c r="G44">
-        <f>H38</f>
+        <f>H38*1000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5677,8 +5677,8 @@
         <v>100.70921985815602</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45:G47" si="9">H39</f>
-        <v>200</v>
+        <f t="shared" ref="G45:G47" si="9">H39*1000000</f>
+        <v>200000000</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -5692,7 +5692,7 @@
       </c>
       <c r="G46">
         <f t="shared" si="9"/>
-        <v>400</v>
+        <v>400000000</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -5705,8 +5705,8 @@
         <v>600</v>
       </c>
       <c r="G47">
-        <f t="shared" si="9"/>
-        <v>464.82758620689663</v>
+        <f>H41*1000000</f>
+        <v>464827586.2068966</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.2">
@@ -5724,7 +5724,7 @@
       </c>
       <c r="F50">
         <f>LOG(1000000*G45)</f>
-        <v>8.3010299956639813</v>
+        <v>14.301029995663981</v>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.2">
@@ -5734,7 +5734,7 @@
       </c>
       <c r="F51">
         <f t="shared" ref="F51:F52" si="11">LOG(1000000*G46)</f>
-        <v>8.6020599913279625</v>
+        <v>14.602059991327963</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.2">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="11"/>
-        <v>8.6672918943003445</v>
+        <v>14.667291894300345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add calculation of capacity in MWe
</commit_message>
<xml_diff>
--- a/data/desalination_costs.xlsx
+++ b/data/desalination_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Projects/Kenya2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6484F246-BEEC-E447-BC47-4D52E89CF832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE005AB-7F9C-084A-AEEB-952DCAA51E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="-940" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>County</t>
   </si>
@@ -190,18 +190,28 @@
   <si>
     <t>log(CAPEX $)</t>
   </si>
+  <si>
+    <t>Size (MWe)</t>
+  </si>
+  <si>
+    <t>Electricity consumption</t>
+  </si>
+  <si>
+    <t>MWhe/m3-H2O</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_)&quot; GWh&quot;;_(* \(#,##0\)&quot; GWh&quot;;_(* &quot;-&quot;??_)&quot; GWh&quot;;_(@_)&quot; GWh&quot;"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_)&quot; MW&quot;;_(* \(#,##0\)&quot; MW&quot;;_(* &quot;-&quot;??_)&quot; MW&quot;;_(@_)&quot; MW&quot;"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -278,7 +288,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -312,6 +322,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1921,7 +1932,7 @@
                   <c:v>0.60052808680521508</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77508201865596704</c:v>
+                  <c:v>0.77508201865596715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4469,15 +4480,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>603251</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>1111251</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>116115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>539751</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>376465</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1815</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5314,8 +5325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C8F88-4382-4F4A-9CA7-C097F9CC2787}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5424,6 +5435,18 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>3.2499999999999999E-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
@@ -5438,6 +5461,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="21">
+        <f>$B$7*E8</f>
+        <v>2.6859504132231402</v>
+      </c>
       <c r="E8" s="19">
         <f>F8*1000000/(24*1000)</f>
         <v>826.44628099173553</v>
@@ -5456,12 +5483,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="21">
+        <f t="shared" ref="D9:D11" si="0">$B$7*E9</f>
+        <v>10.296143250688706</v>
+      </c>
       <c r="E9" s="19">
         <f>F9*1000000/(24*1000)</f>
         <v>3168.0440771349868</v>
       </c>
       <c r="F9" s="18">
-        <f t="shared" ref="F9:F11" si="0">F3</f>
+        <f t="shared" ref="F9:F11" si="1">F3</f>
         <v>76.033057851239676</v>
       </c>
       <c r="G9">
@@ -5474,38 +5505,46 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="21">
+        <f t="shared" si="0"/>
+        <v>41.408402203856753</v>
+      </c>
       <c r="E10" s="19">
         <f>F10*1000000/(24*1000)</f>
         <v>12741.046831955924</v>
       </c>
       <c r="F10" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>305.78512396694219</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G11" si="1">H4*1000000</f>
+        <f t="shared" ref="G10:G11" si="2">H4*1000000</f>
         <v>40000000</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H9:H11" si="2">G10*(1-0.41)</f>
+        <f t="shared" ref="H10:H11" si="3">G10*(1-0.41)</f>
         <v>23600000.000000004</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D11" s="21">
+        <f t="shared" si="0"/>
+        <v>81.25</v>
+      </c>
       <c r="E11" s="19">
         <f>F11*1000000/(24*1000)</f>
         <v>25000</v>
       </c>
       <c r="F11" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50000000</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29500000.000000004</v>
       </c>
     </row>
@@ -5519,7 +5558,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E14">
-        <f>LOG(E9/$E$9)</f>
+        <f>LOG(D9/$D$9)</f>
         <v>0</v>
       </c>
       <c r="F14">
@@ -5529,21 +5568,21 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E15">
-        <f t="shared" ref="E15:E16" si="3">LOG(E10/$E$9)</f>
+        <f t="shared" ref="E15:E16" si="4">LOG(D10/$D$9)</f>
         <v>0.60441389672143964</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F16" si="4">LOG(H10*1000000)</f>
+        <f t="shared" ref="F15:F16" si="5">LOG(H10*1000000)</f>
         <v>13.372912002970107</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.89714879335453834</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13.469822015978163</v>
       </c>
     </row>
@@ -5599,7 +5638,7 @@
         <v>0.71</v>
       </c>
       <c r="F39" s="18">
-        <f t="shared" ref="F39:F40" si="5">$B$38*E39</f>
+        <f t="shared" ref="F39:F40" si="6">$B$38*E39</f>
         <v>100.70921985815602</v>
       </c>
       <c r="G39">
@@ -5615,11 +5654,11 @@
         <v>2.83</v>
       </c>
       <c r="F40" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>401.41843971631209</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40" si="6">H40/$B$39</f>
+        <f t="shared" ref="G40" si="7">H40/$B$39</f>
         <v>2.9</v>
       </c>
       <c r="H40">
@@ -5643,6 +5682,9 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
       <c r="E43" t="s">
         <v>46</v>
       </c>
@@ -5654,6 +5696,10 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D44" s="21">
+        <f>E44*$B$7</f>
+        <v>3.6495271867612291</v>
+      </c>
       <c r="E44">
         <f>F44*1000000/(24*1000)</f>
         <v>1122.9314420803782</v>
@@ -5668,40 +5714,52 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D45" s="21">
+        <f t="shared" ref="D45:D47" si="8">E45*$B$7</f>
+        <v>13.63770685579196</v>
+      </c>
       <c r="E45">
-        <f t="shared" ref="E45:E47" si="7">F45*1000000/(24*1000)</f>
+        <f>F45*1000000/(24*1000)</f>
         <v>4196.217494089834</v>
       </c>
       <c r="F45" s="18">
-        <f t="shared" ref="F45:F47" si="8">F39</f>
+        <f t="shared" ref="F45:F47" si="9">F39</f>
         <v>100.70921985815602</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45:G47" si="9">H39*1000000</f>
+        <f t="shared" ref="G45:G46" si="10">H39*1000000</f>
         <v>200000000</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D46" s="21">
+        <f t="shared" si="8"/>
+        <v>54.358747044917266</v>
+      </c>
       <c r="E46">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E45:E47" si="11">F46*1000000/(24*1000)</f>
         <v>16725.768321513006</v>
       </c>
       <c r="F46" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>401.41843971631209</v>
       </c>
       <c r="G46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>400000000</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D47" s="21">
+        <f t="shared" si="8"/>
+        <v>81.25</v>
+      </c>
       <c r="E47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>25000</v>
       </c>
       <c r="F47" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>600</v>
       </c>
       <c r="G47">
@@ -5719,7 +5777,7 @@
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E50">
-        <f>LOG(E45/$E$45)</f>
+        <f>LOG(D45/$D$45)</f>
         <v>0</v>
       </c>
       <c r="F50">
@@ -5729,21 +5787,21 @@
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E51">
-        <f t="shared" ref="E51:E52" si="10">LOG(E46/$E$45)</f>
+        <f t="shared" ref="E51:E52" si="12">LOG(D46/$D$45)</f>
         <v>0.60052808680521508</v>
       </c>
       <c r="F51">
-        <f t="shared" ref="F51:F52" si="11">LOG(1000000*G46)</f>
+        <f t="shared" ref="F51:F52" si="13">LOG(1000000*G46)</f>
         <v>14.602059991327963</v>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E52">
-        <f t="shared" si="10"/>
-        <v>0.77508201865596704</v>
+        <f t="shared" si="12"/>
+        <v>0.77508201865596715</v>
       </c>
       <c r="F52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>14.667291894300345</v>
       </c>
     </row>
@@ -5754,6 +5812,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009C96272D6B1C1248BA61F90272C32260" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="531a93ae3a83a115bbeb49669be066cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9af1e83-57e1-45b2-b43e-822085829100" xmlns:ns3="b944ac21-af7d-4017-a20b-3a18ec0067d2" xmlns:ns4="ca77b916-f394-4de9-b274-c15ee8638632" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a47a8a0d46cc54d4d61d50ae418c7173" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f9af1e83-57e1-45b2-b43e-822085829100"/>
@@ -5975,16 +6042,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F468DC-AC80-4B5C-9AC0-51BC70A5681A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B894BA-BC54-47C5-9238-FF5A8BF3718F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6002,12 +6068,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F468DC-AC80-4B5C-9AC0-51BC70A5681A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>